<commit_message>
**Étlap feltöltés front-endről** +Lemondás chipsek
</commit_message>
<xml_diff>
--- a/server/etlap5.xlsx
+++ b/server/etlap5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FoodE2.0\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D925107-C76B-44F7-99C4-87342E682791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40FB8C6-D09C-4FC5-9300-1FD057D3ABF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="2700" windowWidth="17775" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="254">
   <si>
     <r>
       <rPr>
@@ -2734,9 +2734,6 @@
       </rPr>
       <t>1,5,6,7,8</t>
     </r>
-  </si>
-  <si>
-    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -2967,6 +2964,147 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2996,147 +3134,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3161,7 +3158,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>14223</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>40386</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="437400" cy="293370"/>
@@ -3526,1985 +3523,1980 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.21875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" customWidth="1"/>
-    <col min="5" max="5" width="3.77734375" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" customWidth="1"/>
     <col min="6" max="6" width="4" customWidth="1"/>
     <col min="7" max="7" width="3.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.5546875" customWidth="1"/>
-    <col min="9" max="9" width="4.21875" customWidth="1"/>
-    <col min="10" max="10" width="3.109375" customWidth="1"/>
-    <col min="11" max="11" width="3.77734375" customWidth="1"/>
+    <col min="8" max="8" width="3.5" customWidth="1"/>
+    <col min="9" max="9" width="4.1640625" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" customWidth="1"/>
+    <col min="11" max="11" width="3.83203125" customWidth="1"/>
     <col min="12" max="12" width="4" customWidth="1"/>
     <col min="13" max="13" width="3.33203125" customWidth="1"/>
-    <col min="14" max="14" width="3.5546875" customWidth="1"/>
+    <col min="14" max="14" width="3.5" customWidth="1"/>
     <col min="15" max="15" width="4" customWidth="1"/>
     <col min="16" max="16" width="3.33203125" customWidth="1"/>
-    <col min="17" max="17" width="3.77734375" customWidth="1"/>
+    <col min="17" max="17" width="3.83203125" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="19" max="19" width="3.109375" customWidth="1"/>
-    <col min="20" max="20" width="3.77734375" customWidth="1"/>
+    <col min="19" max="19" width="3.1640625" customWidth="1"/>
+    <col min="20" max="20" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H1" t="s">
-        <v>254</v>
-      </c>
+    <row r="1" spans="1:20" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="59"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="59"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="62"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="65"/>
+      <c r="T1" s="66"/>
     </row>
-    <row r="2" spans="1:20" ht="10.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="11" t="s">
+    <row r="2" spans="1:20" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="28"/>
+      <c r="T2" s="29"/>
+    </row>
+    <row r="3" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="31"/>
+      <c r="T3" s="32"/>
+    </row>
+    <row r="4" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="35"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="42"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+    </row>
+    <row r="9" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="28"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="S10" s="22"/>
+      <c r="T10" s="23"/>
+    </row>
+    <row r="11" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M11" s="31"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="S11" s="31"/>
+      <c r="T11" s="32"/>
+    </row>
+    <row r="12" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="42"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="54">
         <v>1</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="18"/>
-      <c r="T2" s="19"/>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54"/>
     </row>
-    <row r="3" spans="1:20" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="23" t="s">
+    <row r="17" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="16"/>
+    </row>
+    <row r="18" spans="1:20" ht="45.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="S3" s="30"/>
-      <c r="T3" s="31"/>
+      <c r="C18" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="45"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="28"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="M18" s="28"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="S18" s="50"/>
+      <c r="T18" s="51"/>
     </row>
-    <row r="4" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="33"/>
-      <c r="T4" s="34"/>
+    <row r="19" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="17"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="J19" s="31"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="M19" s="31"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="S19" s="31"/>
+      <c r="T19" s="32"/>
     </row>
-    <row r="5" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="2" t="s">
+    <row r="20" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="17"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="O20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="S20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="T20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="5" t="s">
+    <row r="21" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="17"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="S21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="T21" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="17"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="R23" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="35"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="M24" s="42"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+    </row>
+    <row r="25" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="16"/>
+    </row>
+    <row r="26" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="28"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="J26" s="37"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="M26" s="28"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="39" t="s">
+        <v>165</v>
+      </c>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="S26" s="37"/>
+      <c r="T26" s="38"/>
+    </row>
+    <row r="27" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="17"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" s="31"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="M27" s="31"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="32"/>
+      <c r="R27" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="S27" s="31"/>
+      <c r="T27" s="32"/>
+    </row>
+    <row r="28" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T28" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="17"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>39</v>
+      <c r="G29" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q29" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="R29" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="T29" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="2" t="s">
+    <row r="30" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="M30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="N30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="P30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="R30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="T30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="5" t="s">
+    <row r="31" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="S31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="T31" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="35"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="M32" s="42"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+    </row>
+    <row r="33" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="16"/>
+    </row>
+    <row r="34" spans="1:20" ht="51.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G34" s="22"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="J34" s="25"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="M34" s="22"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="S34" s="28"/>
+      <c r="T34" s="29"/>
+    </row>
+    <row r="35" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="17"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" s="31"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="G35" s="31"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="J35" s="31"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="30" t="s">
+        <v>214</v>
+      </c>
+      <c r="M35" s="31"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="32"/>
+      <c r="R35" s="30" t="s">
+        <v>216</v>
+      </c>
+      <c r="S35" s="31"/>
+      <c r="T35" s="32"/>
+    </row>
+    <row r="36" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T36" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="O37" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="R37" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="S37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="T37" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="17"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R38" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="17"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>58</v>
+      <c r="E39" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="O39" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="P39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="S39" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="T39" s="5" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="35">
-        <v>1.7</v>
-      </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="30" t="s">
+    <row r="40" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="G40" s="34"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="M40" s="12"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="35">
-        <v>1.7</v>
-      </c>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-    </row>
-    <row r="10" spans="1:20" ht="7.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="37"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="38"/>
-      <c r="T10" s="39"/>
-    </row>
-    <row r="11" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="J11" s="30"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="S11" s="27"/>
-      <c r="T11" s="28"/>
-    </row>
-    <row r="12" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="M12" s="33"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="34"/>
-      <c r="R12" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="S12" s="33"/>
-      <c r="T12" s="34"/>
-    </row>
-    <row r="13" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="N14" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T15" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q16" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="R16" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="M17" s="36"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="35">
-        <v>1.7</v>
-      </c>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="46">
-        <v>1</v>
-      </c>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-    </row>
-    <row r="18" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="39"/>
-    </row>
-    <row r="19" spans="1:20" ht="45.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="J19" s="30"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="M19" s="30"/>
-      <c r="N19" s="31"/>
-      <c r="O19" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="S19" s="51"/>
-      <c r="T19" s="52"/>
-    </row>
-    <row r="20" spans="1:20" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="J20" s="33"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="M20" s="33"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="S20" s="33"/>
-      <c r="T20" s="34"/>
-    </row>
-    <row r="21" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="S22" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="M24" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="P24" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q24" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="S24" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="T24" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="54" t="s">
-        <v>157</v>
-      </c>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="M25" s="36"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="48" t="s">
-        <v>159</v>
-      </c>
-      <c r="P25" s="48"/>
-      <c r="Q25" s="48"/>
-      <c r="R25" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-    </row>
-    <row r="26" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="38"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="37"/>
-      <c r="S26" s="38"/>
-      <c r="T26" s="39"/>
-    </row>
-    <row r="27" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="55" t="s">
-        <v>161</v>
-      </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="58" t="s">
-        <v>163</v>
-      </c>
-      <c r="J27" s="59"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="M27" s="30"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="61" t="s">
-        <v>165</v>
-      </c>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="58" t="s">
-        <v>166</v>
-      </c>
-      <c r="S27" s="59"/>
-      <c r="T27" s="60"/>
-    </row>
-    <row r="28" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="J28" s="33"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="M28" s="33"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="S28" s="33"/>
-      <c r="T28" s="34"/>
-    </row>
-    <row r="29" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="M30" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="N30" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="P30" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q30" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="R30" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="T30" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R31" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T31" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="O32" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q32" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="R32" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="S32" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="T32" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="36" t="s">
-        <v>202</v>
-      </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="48" t="s">
-        <v>203</v>
-      </c>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="M33" s="36"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="35">
-        <v>1.7</v>
-      </c>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35">
-        <v>1.7</v>
-      </c>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
-    </row>
-    <row r="34" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="37"/>
-      <c r="M34" s="38"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="37"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="37"/>
-      <c r="S34" s="38"/>
-      <c r="T34" s="39"/>
-    </row>
-    <row r="35" spans="1:20" ht="51.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="26" t="s">
-        <v>206</v>
-      </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="55" t="s">
-        <v>207</v>
-      </c>
-      <c r="J35" s="56"/>
-      <c r="K35" s="57"/>
-      <c r="L35" s="26" t="s">
-        <v>208</v>
-      </c>
-      <c r="M35" s="27"/>
-      <c r="N35" s="28"/>
-      <c r="O35" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="31"/>
-      <c r="R35" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="S35" s="30"/>
-      <c r="T35" s="31"/>
-    </row>
-    <row r="36" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="32" t="s">
-        <v>212</v>
-      </c>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="J36" s="33"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="M36" s="33"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="34"/>
-      <c r="R36" s="32" t="s">
-        <v>216</v>
-      </c>
-      <c r="S36" s="33"/>
-      <c r="T36" s="34"/>
-    </row>
-    <row r="37" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P37" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q37" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T37" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="L38" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="N38" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="O38" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="P38" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q38" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="R38" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="S38" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="T38" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R39" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="S39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T39" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="K40" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="L40" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="N40" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="O40" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="P40" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="R40" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="S40" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="T40" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="66" t="s">
-        <v>250</v>
-      </c>
-      <c r="G41" s="66"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="65" t="s">
-        <v>251</v>
-      </c>
-      <c r="J41" s="65"/>
-      <c r="K41" s="65"/>
-      <c r="L41" s="67" t="s">
-        <v>252</v>
-      </c>
-      <c r="M41" s="67"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="65" t="s">
-        <v>60</v>
-      </c>
-      <c r="P41" s="65"/>
-      <c r="Q41" s="65"/>
-      <c r="R41" s="67" t="s">
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S41" s="67"/>
-      <c r="T41" s="67"/>
+      <c r="S40" s="12"/>
+      <c r="T40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="130">
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="R41:T41"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="R33:T33"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="R9:T9"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="L11:N11"/>
+    <mergeCell ref="O11:Q11"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="A18:A24"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L19:N19"/>
+    <mergeCell ref="O19:Q19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="O24:Q24"/>
+    <mergeCell ref="R24:T24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="O25:Q25"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="O27:Q27"/>
+    <mergeCell ref="R27:T27"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:B40"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="F34:H34"/>
     <mergeCell ref="I34:K34"/>
     <mergeCell ref="L34:N34"/>
     <mergeCell ref="O34:Q34"/>
     <mergeCell ref="R34:T34"/>
-    <mergeCell ref="A35:A41"/>
-    <mergeCell ref="B35:B41"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="L35:N35"/>
     <mergeCell ref="O35:Q35"/>
     <mergeCell ref="R35:T35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="O36:Q36"/>
-    <mergeCell ref="R36:T36"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="O27:Q27"/>
-    <mergeCell ref="R27:T27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="O28:Q28"/>
-    <mergeCell ref="R28:T28"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="O40:Q40"/>
+    <mergeCell ref="R40:T40"/>
+    <mergeCell ref="O32:Q32"/>
+    <mergeCell ref="R32:T32"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="I33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L19:N19"/>
-    <mergeCell ref="O19:Q19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="O25:Q25"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="R9:T9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="O11:Q11"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="L12:N12"/>
-    <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L33:N33"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="R33:T33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>